<commit_message>
Add family and capacity to SKU column. Clean-up output.
</commit_message>
<xml_diff>
--- a/SampleOutput.xlsx
+++ b/SampleOutput.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\acrp2acre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2407F4B-8887-4D8E-80AC-62FC00CA1D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E180A767-C1DF-4F90-A437-575C7A19FF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-2190" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Subscription ID</t>
   </si>
@@ -52,28 +52,22 @@
     <t>Max Total Connections</t>
   </si>
   <si>
-    <t>04a9ce47-b2fd-4461-a841-787c6192ceb8</t>
-  </si>
-  <si>
-    <t>Basic</t>
-  </si>
-  <si>
-    <t>Premium</t>
-  </si>
-  <si>
-    <t>Standard</t>
+    <t>C0 Basic</t>
+  </si>
+  <si>
+    <t>P1 Premium</t>
   </si>
   <si>
     <t>demo-rg</t>
   </si>
   <si>
-    <t>demo-basic</t>
-  </si>
-  <si>
-    <t>demo-premium</t>
-  </si>
-  <si>
-    <t>demo-standard-2</t>
+    <t>demo-1</t>
+  </si>
+  <si>
+    <t>demo-2</t>
+  </si>
+  <si>
+    <t>00000000-0000-0000-0000-000000000000</t>
   </si>
 </sst>
 </file>
@@ -441,18 +435,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.19921875" customWidth="1"/>
-    <col min="3" max="3" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.46484375" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.86328125" bestFit="1" customWidth="1"/>
@@ -495,16 +489,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -516,173 +510,109 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>44042</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>132.66</v>
+        <v>0.7</v>
       </c>
       <c r="J2">
-        <v>62</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>52999</v>
+        <v>36</v>
       </c>
       <c r="I3">
-        <v>897.1</v>
+        <v>4568.99</v>
       </c>
       <c r="J3">
-        <v>93</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>53135</v>
+        <v>28</v>
       </c>
       <c r="I4">
-        <v>902.28</v>
+        <v>4569.54</v>
       </c>
       <c r="J4">
-        <v>65</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5">
-        <v>47023</v>
+        <v>44</v>
       </c>
       <c r="I5">
-        <v>559.11</v>
+        <v>4571.0600000000004</v>
       </c>
       <c r="J5">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>49812</v>
-      </c>
-      <c r="I6">
-        <v>555.34</v>
-      </c>
-      <c r="J6">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>13695</v>
-      </c>
-      <c r="I7">
-        <v>106.43</v>
-      </c>
-      <c r="J7">
-        <v>65</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split SKU capacity and family into separate columns
</commit_message>
<xml_diff>
--- a/SampleOutput.xlsx
+++ b/SampleOutput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\acrp2acre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E180A767-C1DF-4F90-A437-575C7A19FF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01B46A2-09E8-4679-908A-8F0C5E68E293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-2190" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Subscription ID</t>
   </si>
@@ -31,9 +31,6 @@
     <t>DB Name</t>
   </si>
   <si>
-    <t>SKU</t>
-  </si>
-  <si>
     <t>Replicas per Master</t>
   </si>
   <si>
@@ -52,12 +49,6 @@
     <t>Max Total Connections</t>
   </si>
   <si>
-    <t>C0 Basic</t>
-  </si>
-  <si>
-    <t>P1 Premium</t>
-  </si>
-  <si>
     <t>demo-rg</t>
   </si>
   <si>
@@ -68,6 +59,24 @@
   </si>
   <si>
     <t>00000000-0000-0000-0000-000000000000</t>
+  </si>
+  <si>
+    <t>SKU Capacity</t>
+  </si>
+  <si>
+    <t>SKU Name</t>
+  </si>
+  <si>
+    <t>C0</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Premium</t>
   </si>
 </sst>
 </file>
@@ -435,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -446,16 +455,17 @@
     <col min="1" max="1" width="34.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.46484375" customWidth="1"/>
-    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,152 +476,167 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>0.7</v>
+      </c>
+      <c r="K2">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="I3">
+        <v>36</v>
+      </c>
+      <c r="J3">
+        <v>4568.99</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>0.7</v>
-      </c>
-      <c r="J2">
-        <v>19</v>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>28</v>
+      </c>
+      <c r="J4">
+        <v>4569.54</v>
+      </c>
+      <c r="K4">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>36</v>
-      </c>
-      <c r="I3">
-        <v>4568.99</v>
-      </c>
-      <c r="J3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>28</v>
-      </c>
-      <c r="I4">
-        <v>4569.54</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>44</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>4571.0600000000004</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>8</v>
       </c>
     </row>

</xml_diff>